<commit_message>
Update 조의호님 20년납30세만기 47.410원.xlsx
</commit_message>
<xml_diff>
--- a/3. 자료/보험_콩떡이/조의호님 20년납30세만기 47.410원.xlsx
+++ b/3. 자료/보험_콩떡이/조의호님 20년납30세만기 47.410원.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Study\3. 자료\보험_콩떡이\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Study\3. 자료\보험_콩떡이\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A381B4D6-BF5F-44AF-9B70-27405D34A0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$76</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -372,7 +373,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -464,31 +465,31 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,7 +504,7 @@
     <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -525,9 +526,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -565,9 +566,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,7 +603,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,7 +638,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -810,11 +811,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+      <selection activeCell="F73" sqref="F2:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -2648,8 +2649,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G76">
-    <sortState ref="A2:G76">
+  <autoFilter ref="A1:G76" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G76">
       <sortCondition ref="A1:A76"/>
     </sortState>
   </autoFilter>

</xml_diff>